<commit_message>
upload before fork branch
</commit_message>
<xml_diff>
--- a/spec/IMPD_X30_Unit_Test_Specification (version 1).xlsb.xlsx
+++ b/spec/IMPD_X30_Unit_Test_Specification (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\long.trinh-tien\Documents\Git\training_ut_it_Long\spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1074231-6FA2-4979-9D1E-AA685CE02455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8757ED0B-D684-4D1F-9A62-F6215C44FFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{98A04C18-7F5B-4AE7-A401-12E90007D75B}"/>
   </bookViews>
@@ -676,7 +676,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2938" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2938" uniqueCount="290">
   <si>
     <t>&lt;=Summary</t>
   </si>
@@ -1634,6 +1634,9 @@
   </si>
   <si>
     <t>unknown core state</t>
+  </si>
+  <si>
+    <t>not stub</t>
   </si>
 </sst>
 </file>
@@ -11496,10 +11499,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:W41"/>
+  <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="N10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11" outlineLevelCol="1"/>
@@ -12178,10 +12181,10 @@
         <v>0</v>
       </c>
       <c r="U15" s="68" t="s">
-        <v>132</v>
+        <v>289</v>
       </c>
       <c r="V15" s="68" t="s">
-        <v>132</v>
+        <v>289</v>
       </c>
       <c r="W15" s="68" t="s">
         <v>131</v>
@@ -13149,19 +13152,16 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="2:23" ht="15" customHeight="1">
+    <row r="30" spans="2:23" ht="13.5" customHeight="1">
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="2:23" ht="13.5" customHeight="1">
+    <row r="31" spans="2:23" ht="15" customHeight="1">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="2:23" ht="15" customHeight="1">
-      <c r="B32" s="7"/>
-    </row>
-    <row r="41" spans="6:8">
-      <c r="F41" s="73"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="73"/>
+    <row r="40" spans="6:8">
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -15125,8 +15125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03D3585-9FCD-4938-B4DD-F07BF8EF78E3}">
   <dimension ref="A1:Y88"/>
   <sheetViews>
-    <sheetView topLeftCell="C60" workbookViewId="0">
-      <selection activeCell="C74" sqref="A74:XFD74"/>
+    <sheetView topLeftCell="C45" workbookViewId="0">
+      <selection activeCell="C73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
add delete 1 func obj, update tasks.json
</commit_message>
<xml_diff>
--- a/spec/IMPD_X30_Unit_Test_Specification (version 1).xlsb.xlsx
+++ b/spec/IMPD_X30_Unit_Test_Specification (version 1).xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\long.trinh-tien\Documents\Git\training_ut_it_Long\spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5CE4B3-FFED-4C92-A3D8-6FE670639DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99654341-5C62-47DA-A907-AB2CA18FFCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{98A04C18-7F5B-4AE7-A401-12E90007D75B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{98A04C18-7F5B-4AE7-A401-12E90007D75B}"/>
   </bookViews>
   <sheets>
     <sheet name="R_IMPDRV_GetPMPolicy" sheetId="2" r:id="rId1"/>
@@ -14878,8 +14878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4151AE-3DD6-47AB-BAF1-B146FD01F5F4}">
   <dimension ref="A1:AK57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11" outlineLevelCol="1"/>

</xml_diff>